<commit_message>
Change test to use AppKeys.xlsx for API key and secret key.
</commit_message>
<xml_diff>
--- a/ops/config/AppKeys.xlsx
+++ b/ops/config/AppKeys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenlooplee\Documents\GitHub\BaiduOcrActivitiesPack\ops\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B54D5A1-E3D2-493C-865B-970089516062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E9C80C-9BD9-460A-8640-D50AF8733CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18436" windowHeight="11160" xr2:uid="{D6D768DA-5964-4C9E-A98A-0598DDF1AEA9}"/>
   </bookViews>
@@ -53,10 +53,10 @@
     <t>SecretKey</t>
   </si>
   <si>
-    <t>AppName1</t>
-  </si>
-  <si>
-    <t>AppDescription1</t>
+    <t>TestApp1</t>
+  </si>
+  <si>
+    <t>Test the creation of an app.</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>